<commit_message>
Re-analysis of AI Feynman Equations with addition of symbolic constant ('one') for 1
</commit_message>
<xml_diff>
--- a/Analysis of AI Feynman Problems.xlsx
+++ b/Analysis of AI Feynman Problems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanlenchner/Documents/Science 2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87948403-655D-2F40-890D-A5E3D0A07D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D90BC3A-091A-5A42-B4F2-2D2209E84604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1140" yWindow="-18100" windowWidth="34560" windowHeight="20340" xr2:uid="{07C40A93-C0E6-8C46-8FF0-54ED706A0F98}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="26240" windowHeight="16380" xr2:uid="{07C40A93-C0E6-8C46-8FF0-54ED706A0F98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="180">
   <si>
     <t>Feynman Eqn</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Issue</t>
   </si>
   <si>
-    <t>exp()</t>
-  </si>
-  <si>
     <t>I.8.14</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>I.12.11</t>
   </si>
   <si>
-    <t>sin()</t>
-  </si>
-  <si>
     <t>I13. 4</t>
   </si>
   <si>
@@ -131,15 +125,9 @@
     <t>1,3</t>
   </si>
   <si>
-    <t>I.14 . 4</t>
-  </si>
-  <si>
     <t>I.15.3x</t>
   </si>
   <si>
-    <t>I.15 .3t</t>
-  </si>
-  <si>
     <t>I.15.10</t>
   </si>
   <si>
@@ -170,15 +158,9 @@
     <t>1,3,3</t>
   </si>
   <si>
-    <t>I.2 5.13</t>
-  </si>
-  <si>
     <t>I.26.2</t>
   </si>
   <si>
-    <t>arcsin(), sin()</t>
-  </si>
-  <si>
     <t>I.27.6</t>
   </si>
   <si>
@@ -218,9 +200,6 @@
     <t>I.37.4</t>
   </si>
   <si>
-    <t>cos()</t>
-  </si>
-  <si>
     <t>I.38.12</t>
   </si>
   <si>
@@ -299,15 +278,9 @@
     <t>II.6.15b</t>
   </si>
   <si>
-    <t>cos(), sin()</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Really same. eqn as previous one</t>
-  </si>
-  <si>
     <t>I.6.20</t>
   </si>
   <si>
@@ -344,9 +317,6 @@
     <t>II.11.28</t>
   </si>
   <si>
-    <t>1 term</t>
-  </si>
-  <si>
     <t>II.13.17</t>
   </si>
   <si>
@@ -365,12 +335,6 @@
     <t>2,2,4</t>
   </si>
   <si>
-    <t>II.15. 4</t>
-  </si>
-  <si>
-    <t>II.1 5. 5</t>
-  </si>
-  <si>
     <t>II.21.32</t>
   </si>
   <si>
@@ -407,12 +371,6 @@
     <t>II.34.29b</t>
   </si>
   <si>
-    <t>II.3 5.18</t>
-  </si>
-  <si>
-    <t>II.3 5.21</t>
-  </si>
-  <si>
     <t>tanh()</t>
   </si>
   <si>
@@ -485,9 +443,6 @@
     <t>I.29.16</t>
   </si>
   <si>
-    <t>Silly form of the distance formula</t>
-  </si>
-  <si>
     <t>I.30.3</t>
   </si>
   <si>
@@ -509,9 +464,6 @@
     <t>(32)</t>
   </si>
   <si>
-    <t>Essentially the same as previous eqn</t>
-  </si>
-  <si>
     <t>Using 1D Version</t>
   </si>
   <si>
@@ -534,6 +486,96 @@
   </si>
   <si>
     <t>Fit Our Model?</t>
+  </si>
+  <si>
+    <t>Uses exp()</t>
+  </si>
+  <si>
+    <t>Uses sin()</t>
+  </si>
+  <si>
+    <t>1,2,4</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>Uses cos()</t>
+  </si>
+  <si>
+    <t>1,1,1,3</t>
+  </si>
+  <si>
+    <t>Uses sin^2()</t>
+  </si>
+  <si>
+    <t>Uses cos^2)_</t>
+  </si>
+  <si>
+    <t>1,1,1,4</t>
+  </si>
+  <si>
+    <t>2,3,4</t>
+  </si>
+  <si>
+    <t>1,2,2</t>
+  </si>
+  <si>
+    <t>2,5</t>
+  </si>
+  <si>
+    <t>Uses sin(), cos()</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>3,3,3</t>
+  </si>
+  <si>
+    <t>Simplifies to theta = 1 + n*alpha</t>
+  </si>
+  <si>
+    <t>II.35.18</t>
+  </si>
+  <si>
+    <t>II.35.21</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>Uses sin() - argument to sin() becomes a new variable</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>1,1,2</t>
+  </si>
+  <si>
+    <t>1,1,3</t>
+  </si>
+  <si>
+    <t>I.14.4</t>
+  </si>
+  <si>
+    <t>I.15.3t</t>
+  </si>
+  <si>
+    <t>I.25.13</t>
+  </si>
+  <si>
+    <t>II.15.4</t>
+  </si>
+  <si>
+    <t>II.15.5</t>
+  </si>
+  <si>
+    <t>1,1,2,2,3</t>
+  </si>
+  <si>
+    <t>Uses exp() - argument to exp() becomes a new variable</t>
   </si>
 </sst>
 </file>
@@ -656,7 +698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -673,19 +715,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1034,9 +1073,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBEB1909-1A74-5840-9B5A-449C438F86C1}">
   <dimension ref="A1:T118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="162" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="162" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q99" sqref="Q99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1062,10 +1101,10 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G1" s="1" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
@@ -1079,7 +1118,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
@@ -1125,63 +1164,111 @@
         <v>6</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>157</v>
+        <v>150</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <v>1</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -1198,16 +1285,16 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -1224,16 +1311,16 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8">
         <v>3</v>
@@ -1244,19 +1331,19 @@
     </row>
     <row r="9" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1270,16 +1357,16 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1293,16 +1380,16 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1319,16 +1406,16 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12" t="s">
-        <v>22</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1345,53 +1432,71 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
       <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>152</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1408,16 +1513,16 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16">
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -1431,16 +1536,16 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17">
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1454,16 +1559,16 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18">
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1480,16 +1585,16 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19">
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H19">
         <v>3</v>
@@ -1506,16 +1611,16 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>174</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20">
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H20">
         <v>3</v>
@@ -1532,16 +1637,16 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E21">
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21">
         <v>3</v>
@@ -1552,16 +1657,16 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22">
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H22">
         <v>3</v>
@@ -1575,16 +1680,16 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23">
         <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H23">
         <v>4</v>
@@ -1593,40 +1698,70 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>153</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26">
         <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -1643,16 +1778,16 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>175</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1666,27 +1801,27 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E29">
         <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H29">
         <v>2</v>
@@ -1700,16 +1835,16 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E30">
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -1721,54 +1856,81 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>155</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>3</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>108</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="N32">
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E34">
         <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -1785,16 +1947,16 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E35">
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -1814,16 +1976,16 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36">
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -1837,16 +1999,16 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E37">
         <v>3</v>
       </c>
       <c r="F37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H37">
         <v>3</v>
@@ -1857,16 +2019,16 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E38">
         <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -1883,16 +2045,16 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E39">
         <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -1904,29 +2066,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" t="s">
-        <v>60</v>
+        <v>9</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40" t="s">
+        <v>158</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>3</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E41">
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="I41">
         <v>2</v>
@@ -1940,16 +2120,16 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E42">
         <v>2</v>
       </c>
       <c r="F42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -1966,16 +2146,16 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E43">
         <v>3</v>
       </c>
       <c r="F43" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -1989,16 +2169,16 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E44">
         <v>2</v>
       </c>
       <c r="F44" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -2010,40 +2190,73 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46" t="s">
+        <v>159</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E47">
         <v>2</v>
       </c>
       <c r="F47" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -2057,16 +2270,16 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E48">
         <v>2</v>
       </c>
       <c r="F48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -2080,16 +2293,16 @@
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E49">
         <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H49">
         <v>2</v>
@@ -2103,27 +2316,27 @@
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B50" t="s">
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E51">
         <v>2</v>
       </c>
       <c r="F51" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -2137,16 +2350,16 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E52">
         <v>3</v>
       </c>
       <c r="F52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H52">
         <v>3</v>
@@ -2155,29 +2368,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" t="s">
-        <v>60</v>
+        <v>9</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="F53" t="s">
+        <v>160</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="N53">
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E54">
         <v>3</v>
       </c>
       <c r="F54" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -2191,16 +2419,16 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E55">
         <v>2</v>
       </c>
       <c r="F55" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -2217,16 +2445,16 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E56">
         <v>2</v>
       </c>
       <c r="F56" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -2241,29 +2469,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" t="s">
-        <v>60</v>
+        <v>9</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>161</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <v>1</v>
+      </c>
+      <c r="Q57">
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E58">
         <v>2</v>
       </c>
       <c r="F58" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I58">
         <v>1</v>
@@ -2280,30 +2526,45 @@
     </row>
     <row r="59" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>89</v>
+        <v>162</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59" t="s">
+        <v>163</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="P59">
+        <v>1</v>
+      </c>
+      <c r="Q59">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E60">
         <v>2</v>
       </c>
       <c r="F60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G60">
         <v>1</v>
@@ -2315,21 +2576,21 @@
         <v>1</v>
       </c>
       <c r="T60" s="4" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E61">
         <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -2346,16 +2607,16 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E62">
         <v>3</v>
       </c>
       <c r="F62" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G62">
         <v>1</v>
@@ -2369,16 +2630,16 @@
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E63">
         <v>3</v>
       </c>
       <c r="F63" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="H63">
         <v>1</v>
@@ -2390,29 +2651,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" t="s">
-        <v>60</v>
+        <v>9</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64" t="s">
+        <v>164</v>
+      </c>
+      <c r="I64">
+        <v>3</v>
+      </c>
+      <c r="N64">
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E65">
         <v>2</v>
       </c>
       <c r="F65" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="I65">
         <v>2</v>
@@ -2426,16 +2699,16 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E66">
         <v>3</v>
       </c>
       <c r="F66" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="G66">
         <v>1</v>
@@ -2453,29 +2726,50 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E67">
         <v>5</v>
       </c>
-      <c r="C67" t="s">
-        <v>102</v>
+      <c r="F67" t="s">
+        <v>178</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+      <c r="H67">
+        <v>2</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="N67">
+        <v>2</v>
+      </c>
+      <c r="P67">
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E68">
         <v>2</v>
       </c>
       <c r="F68" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="G68">
         <v>1</v>
@@ -2492,16 +2786,16 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E69">
         <v>3</v>
       </c>
       <c r="F69" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H69">
         <v>2</v>
@@ -2515,16 +2809,16 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E70">
         <v>3</v>
       </c>
       <c r="F70" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H70">
         <v>2</v>
@@ -2536,40 +2830,70 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E71">
+        <v>2</v>
+      </c>
+      <c r="F71" t="s">
+        <v>28</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="N71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" t="s">
-        <v>60</v>
+        <v>9</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="F72" t="s">
+        <v>28</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="N72">
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E73">
         <v>3</v>
       </c>
       <c r="F73" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -2589,16 +2913,16 @@
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B74" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E74">
         <v>3</v>
       </c>
       <c r="F74" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H74">
         <v>2</v>
@@ -2612,16 +2936,16 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E75">
         <v>2</v>
       </c>
       <c r="F75" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G75">
         <v>1</v>
@@ -2635,16 +2959,16 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E76">
         <v>2</v>
       </c>
       <c r="F76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G76">
         <v>1</v>
@@ -2658,16 +2982,16 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E77">
         <v>2</v>
       </c>
       <c r="F77" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -2684,16 +3008,16 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E78">
         <v>2</v>
       </c>
       <c r="F78" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G78">
         <v>1</v>
@@ -2710,16 +3034,16 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E79">
         <v>2</v>
       </c>
       <c r="F79" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="H79">
         <v>2</v>
@@ -2733,16 +3057,16 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E80">
         <v>2</v>
       </c>
       <c r="F80" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -2759,16 +3083,16 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E81">
         <v>2</v>
       </c>
       <c r="F81" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -2782,38 +3106,53 @@
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="D82" t="s">
+        <v>150</v>
+      </c>
+      <c r="E82">
+        <v>3</v>
+      </c>
+      <c r="F82" t="s">
+        <v>160</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <v>2</v>
+      </c>
+      <c r="N82">
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>124</v>
+        <v>167</v>
       </c>
       <c r="B83" t="s">
         <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="B84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E84">
         <v>3</v>
       </c>
       <c r="F84" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="I84">
         <v>1</v>
@@ -2830,16 +3169,16 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E85">
         <v>3</v>
       </c>
       <c r="F85" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="G85">
         <v>1</v>
@@ -2856,16 +3195,16 @@
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E86">
         <v>2</v>
       </c>
       <c r="F86" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -2879,16 +3218,16 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E87">
         <v>3</v>
       </c>
       <c r="F87" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="G87">
         <v>2</v>
@@ -2903,43 +3242,70 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E88">
+        <v>3</v>
+      </c>
+      <c r="F88" t="s">
+        <v>171</v>
+      </c>
+      <c r="G88">
+        <v>2</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="N88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B89" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>89</v>
+        <v>150</v>
+      </c>
+      <c r="E89">
+        <v>3</v>
+      </c>
+      <c r="F89" t="s">
+        <v>160</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89">
+        <v>2</v>
+      </c>
+      <c r="N89">
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E90">
         <v>2</v>
       </c>
       <c r="F90" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G90">
         <v>1</v>
@@ -2954,40 +3320,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E91">
+        <v>2</v>
+      </c>
+      <c r="F91" t="s">
+        <v>168</v>
+      </c>
+      <c r="G91">
+        <v>2</v>
+      </c>
+      <c r="N91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E92">
+        <v>2</v>
+      </c>
+      <c r="F92" t="s">
+        <v>170</v>
+      </c>
+      <c r="I92">
+        <v>1</v>
+      </c>
+      <c r="J92">
+        <v>1</v>
+      </c>
+      <c r="N92">
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E93">
         <v>2</v>
       </c>
       <c r="F93" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G93">
         <v>1</v>
@@ -3001,16 +3394,16 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="B94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E94">
         <v>2</v>
       </c>
       <c r="F94" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G94">
         <v>1</v>
@@ -3024,16 +3417,16 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E95">
         <v>2</v>
       </c>
       <c r="F95" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H95">
         <v>1</v>
@@ -3048,40 +3441,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
-      </c>
-      <c r="C96" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E96">
+        <v>3</v>
+      </c>
+      <c r="F96" t="s">
+        <v>171</v>
+      </c>
+      <c r="G96">
+        <v>2</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="N96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" t="s">
-        <v>60</v>
+        <v>9</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E97">
+        <v>3</v>
+      </c>
+      <c r="F97" t="s">
+        <v>117</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <v>1</v>
+      </c>
+      <c r="N97">
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="B98" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E98">
         <v>2</v>
       </c>
       <c r="F98" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G98">
         <v>1</v>
@@ -3098,16 +3524,16 @@
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E99">
         <v>2</v>
       </c>
       <c r="F99" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="H99">
         <v>1</v>
@@ -3115,30 +3541,51 @@
       <c r="I99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N99">
+        <v>1</v>
+      </c>
+      <c r="O99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" t="s">
-        <v>60</v>
+        <v>9</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E100">
+        <v>3</v>
+      </c>
+      <c r="F100" t="s">
+        <v>172</v>
+      </c>
+      <c r="G100">
+        <v>2</v>
+      </c>
+      <c r="I100">
+        <v>1</v>
+      </c>
+      <c r="N100">
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="B101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E101">
         <v>2</v>
       </c>
       <c r="F101" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="H101">
         <v>1</v>
@@ -3150,21 +3597,21 @@
         <v>1</v>
       </c>
       <c r="T101" s="4" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B102" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E102">
         <v>2</v>
       </c>
       <c r="F102" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="H102">
         <v>1</v>
@@ -3178,68 +3625,68 @@
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="B103" s="7"/>
-      <c r="D103" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E103" s="13"/>
+      <c r="D103" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E103" s="12"/>
       <c r="F103" s="7"/>
-      <c r="M103" s="18"/>
-      <c r="N103" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="O103" s="13"/>
-      <c r="P103" s="13"/>
-      <c r="Q103" s="13"/>
-      <c r="R103" s="13"/>
+      <c r="M103" s="16"/>
+      <c r="N103" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="O103" s="12"/>
+      <c r="P103" s="12"/>
+      <c r="Q103" s="12"/>
+      <c r="R103" s="12"/>
       <c r="S103" s="7"/>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A104" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B104" s="9">
-        <f>COUNTIF(B4:B102,"Yes")</f>
-        <v>70</v>
-      </c>
-      <c r="D104" s="14">
-        <v>2</v>
-      </c>
-      <c r="E104" s="15">
+        <f>COUNTIF(B3:B102,"Yes")</f>
+        <v>96</v>
+      </c>
+      <c r="D104" s="13">
+        <v>2</v>
+      </c>
+      <c r="E104">
         <f>COUNTIF(E$3:E$102,D104)</f>
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="F104" s="9">
         <f>E104/SUM(E$104:E$107)</f>
-        <v>0.6</v>
-      </c>
-      <c r="M104" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="N104" s="15">
-        <f>SUM(N6:N102)</f>
-        <v>139</v>
-      </c>
-      <c r="O104" s="15">
-        <f>SUM(O6:O102)</f>
-        <v>15</v>
-      </c>
-      <c r="P104" s="15">
-        <f>SUM(P6:P102)</f>
-        <v>10</v>
-      </c>
-      <c r="Q104" s="15">
-        <f>SUM(Q6:Q102)</f>
-        <v>9</v>
-      </c>
-      <c r="R104" s="15">
-        <f>SUM(R6:R102)</f>
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="M104" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="N104">
+        <f t="shared" ref="N104:S104" si="0">SUM(N6:N102)</f>
+        <v>196</v>
+      </c>
+      <c r="O104">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="P104">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q104">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="R104">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S104" s="9">
-        <f>SUM(S6:S102)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3249,167 +3696,167 @@
       </c>
       <c r="B105" s="11">
         <f>COUNTIF(B3:B102,"no")</f>
+        <v>4</v>
+      </c>
+      <c r="D105" s="13">
+        <v>3</v>
+      </c>
+      <c r="E105">
+        <f>COUNTIF(E$3:E$102,D105)</f>
         <v>30</v>
-      </c>
-      <c r="D105" s="14">
-        <v>3</v>
-      </c>
-      <c r="E105" s="15">
-        <f>COUNTIF(E$3:E$102,D105)</f>
-        <v>20</v>
       </c>
       <c r="F105" s="9">
         <f>E105/SUM(E$104:E$107)</f>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="M105" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="N105" s="24">
+        <v>0.3125</v>
+      </c>
+      <c r="M105" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="N105" s="21">
         <f>N104/SUM($N104:$Q104)</f>
-        <v>0.80346820809248554</v>
-      </c>
-      <c r="O105" s="24">
-        <f t="shared" ref="O105:Q105" si="0">O104/SUM($N104:$Q104)</f>
-        <v>8.6705202312138727E-2</v>
-      </c>
-      <c r="P105" s="24">
-        <f t="shared" si="0"/>
-        <v>5.7803468208092484E-2</v>
-      </c>
-      <c r="Q105" s="24">
-        <f t="shared" si="0"/>
-        <v>5.2023121387283239E-2</v>
-      </c>
-      <c r="R105" s="24">
-        <f t="shared" ref="R105:S105" si="1">R104/SUM($N104:$S104)</f>
+        <v>0.82008368200836823</v>
+      </c>
+      <c r="O105" s="21">
+        <f t="shared" ref="O105:Q105" si="1">O104/SUM($N104:$Q104)</f>
+        <v>7.1129707112970716E-2</v>
+      </c>
+      <c r="P105" s="21">
+        <f t="shared" si="1"/>
+        <v>5.8577405857740586E-2</v>
+      </c>
+      <c r="Q105" s="21">
+        <f t="shared" si="1"/>
+        <v>5.0209205020920501E-2</v>
+      </c>
+      <c r="R105" s="21">
+        <f t="shared" ref="R105:S105" si="2">R104/SUM($N104:$S104)</f>
         <v>0</v>
       </c>
-      <c r="S105" s="25">
-        <f t="shared" si="1"/>
-        <v>5.7471264367816091E-3</v>
+      <c r="S105" s="22">
+        <f t="shared" si="2"/>
+        <v>4.1666666666666666E-3</v>
       </c>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D106" s="14">
+      <c r="D106" s="13">
         <v>4</v>
       </c>
-      <c r="E106" s="15">
+      <c r="E106">
         <f>COUNTIF(E$3:E$102,D106)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F106" s="9">
         <f>E106/SUM(E$104:E$107)</f>
-        <v>8.5714285714285715E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D107" s="16">
+      <c r="D107" s="14">
         <v>5</v>
       </c>
-      <c r="E107" s="17">
+      <c r="E107" s="15">
         <f>COUNTIF(E$3:E$102,D107)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F107" s="9">
         <f>E107/SUM(E$104:E$107)</f>
-        <v>2.8571428571428571E-2</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="F108" s="18"/>
-      <c r="G108" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="H108" s="13"/>
-      <c r="I108" s="13"/>
-      <c r="J108" s="13"/>
-      <c r="K108" s="13"/>
+      <c r="F108" s="16"/>
+      <c r="G108" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="H108" s="12"/>
+      <c r="I108" s="12"/>
+      <c r="J108" s="12"/>
+      <c r="K108" s="12"/>
       <c r="L108" s="7"/>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.2">
       <c r="F109" s="8"/>
-      <c r="G109" s="20">
+      <c r="G109" s="1">
         <f>G2</f>
         <v>1</v>
       </c>
-      <c r="H109" s="20">
-        <f t="shared" ref="H109:L109" si="2">H2</f>
-        <v>2</v>
-      </c>
-      <c r="I109" s="20">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="J109" s="20">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="K109" s="20">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="L109" s="21">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="F110" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="G110" s="15">
-        <f t="shared" ref="G110:L110" si="3">SUM(G6:G102)</f>
-        <v>33</v>
-      </c>
-      <c r="H110" s="15">
+      <c r="H109" s="1">
+        <f t="shared" ref="H109:L109" si="3">H2</f>
+        <v>2</v>
+      </c>
+      <c r="I109" s="1">
         <f t="shared" si="3"/>
-        <v>82</v>
-      </c>
-      <c r="I110" s="15">
-        <f t="shared" si="3"/>
-        <v>42</v>
-      </c>
-      <c r="J110" s="15">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="K110" s="15">
+        <v>3</v>
+      </c>
+      <c r="J109" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
+      <c r="K109" s="1">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="L109" s="18">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="F110" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="G110">
+        <f t="shared" ref="G110:L110" si="4">SUM(G6:G102)</f>
+        <v>59</v>
+      </c>
+      <c r="H110">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+      <c r="I110">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
+      <c r="J110">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="K110">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
       <c r="L110" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="F111" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="G111" s="17">
+      <c r="F111" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="G111" s="15">
         <f>G110/SUM($G110:$L110)</f>
-        <v>0.1864406779661017</v>
-      </c>
-      <c r="H111" s="17">
-        <f t="shared" ref="H111:L111" si="4">H110/SUM($G110:$L110)</f>
-        <v>0.4632768361581921</v>
-      </c>
-      <c r="I111" s="17">
-        <f t="shared" si="4"/>
-        <v>0.23728813559322035</v>
-      </c>
-      <c r="J111" s="17">
-        <f t="shared" si="4"/>
-        <v>8.4745762711864403E-2</v>
-      </c>
-      <c r="K111" s="17">
-        <f t="shared" si="4"/>
-        <v>2.2598870056497175E-2</v>
+        <v>0.24583333333333332</v>
+      </c>
+      <c r="H111" s="15">
+        <f t="shared" ref="H111:L111" si="5">H110/SUM($G110:$L110)</f>
+        <v>0.41249999999999998</v>
+      </c>
+      <c r="I111" s="15">
+        <f t="shared" si="5"/>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="J111" s="15">
+        <f t="shared" si="5"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="K111" s="15">
+        <f t="shared" si="5"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="L111" s="11">
-        <f t="shared" si="4"/>
-        <v>5.6497175141242938E-3</v>
+        <f t="shared" si="5"/>
+        <v>4.1666666666666666E-3</v>
       </c>
     </row>
     <row r="118" spans="7:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated calculation of basic parameters
</commit_message>
<xml_diff>
--- a/Analysis of AI Feynman Problems.xlsx
+++ b/Analysis of AI Feynman Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanlenchner/Documents/Science 2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D90BC3A-091A-5A42-B4F2-2D2209E84604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE611E37-47CC-3040-8784-E7A93DC7F45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="26240" windowHeight="16380" xr2:uid="{07C40A93-C0E6-8C46-8FF0-54ED706A0F98}"/>
+    <workbookView xWindow="-11180" yWindow="4380" windowWidth="26240" windowHeight="16380" xr2:uid="{07C40A93-C0E6-8C46-8FF0-54ED706A0F98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="181">
   <si>
     <t>Feynman Eqn</t>
   </si>
@@ -576,12 +576,18 @@
   </si>
   <si>
     <t>Uses exp() - argument to exp() becomes a new variable</t>
+  </si>
+  <si>
+    <t>Count Sum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -698,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -737,6 +743,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1073,9 +1082,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBEB1909-1A74-5840-9B5A-449C438F86C1}">
   <dimension ref="A1:T118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="162" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q99" sqref="Q99"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="162" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G111" sqref="G111:L111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,10 +1094,9 @@
     <col min="4" max="4" width="18.1640625" style="3" customWidth="1"/>
     <col min="5" max="6" width="18.1640625" customWidth="1"/>
     <col min="7" max="7" width="5.5" customWidth="1"/>
-    <col min="8" max="9" width="5.1640625" customWidth="1"/>
-    <col min="10" max="10" width="4.83203125" customWidth="1"/>
-    <col min="11" max="11" width="5" customWidth="1"/>
-    <col min="12" max="12" width="4.83203125" customWidth="1"/>
+    <col min="8" max="9" width="5.83203125" customWidth="1"/>
+    <col min="10" max="10" width="5.5" customWidth="1"/>
+    <col min="11" max="12" width="5.33203125" customWidth="1"/>
     <col min="13" max="13" width="6.83203125" customWidth="1"/>
     <col min="14" max="14" width="5.33203125" customWidth="1"/>
     <col min="15" max="15" width="4.6640625" customWidth="1"/>
@@ -3800,6 +3808,9 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
+      <c r="M109" s="1" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.2">
       <c r="F110" s="19" t="s">
@@ -3829,32 +3840,36 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
+      <c r="M110" s="26">
+        <f>SUM(G110:L110)</f>
+        <v>240</v>
+      </c>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.2">
       <c r="F111" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="G111" s="15">
+      <c r="G111" s="24">
         <f>G110/SUM($G110:$L110)</f>
         <v>0.24583333333333332</v>
       </c>
-      <c r="H111" s="15">
+      <c r="H111" s="24">
         <f t="shared" ref="H111:L111" si="5">H110/SUM($G110:$L110)</f>
         <v>0.41249999999999998</v>
       </c>
-      <c r="I111" s="15">
+      <c r="I111" s="24">
         <f t="shared" si="5"/>
         <v>0.22500000000000001</v>
       </c>
-      <c r="J111" s="15">
+      <c r="J111" s="24">
         <f t="shared" si="5"/>
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="K111" s="15">
+      <c r="K111" s="24">
         <f t="shared" si="5"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="L111" s="11">
+      <c r="L111" s="25">
         <f t="shared" si="5"/>
         <v>4.1666666666666666E-3</v>
       </c>

</xml_diff>